<commit_message>
Get daily reddit data: Tue Feb  4 08:10:55 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_09.xlsx
+++ b/data/collected_data/2025_02_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C507"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3508 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1ihcd1f</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>First time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yu0dkvar2he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1ihat88</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>A way to remove acrylics without acetone?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihat88/a_way_to_remove_acrylics_without_acetone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1ihc02i</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>I don’t love my nails and I’m wondering the etiquette for potentially getting them changed</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/osxrr3qjm2he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1ih7zuu</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>UV gel help</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih7zuu</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1ihc2cf</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>beginner level bling ?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihc2cf</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1ih9dkx</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Please help, cannot get my nails to grow thicker</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ih9dkx/please_help_cannot_get_my_nails_to_grow_thicker/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1iha38l</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Nail retention help</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iha38l/nail_retention_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1ihbaix</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>What is happening to my nails?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihbaix</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1ihbv23</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>what service(s) are required for these nails? (picture from Pinterest by hyousuta)</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kewvyblpk2he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1ihb2cu</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Good? Bad?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihb2cu</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1ihb1qh</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Non toxic nail polish</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihb1qh/non_toxic_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1ihamkj</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Glue on nail</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihamkj/glue_on_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1iha904</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Retention help</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iha904/retention_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1ih9xo9</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>My first time doing gel extensions and nail art, how to shape better?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih9xo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1ih9erm</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Which set for engagement?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih9erm</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1ih97ht</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Cheese grater caught my nail, what should I do?</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36cpyxuvr1he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1ih9428</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Valentine Nails</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emhp770zq1he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1ih93be</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>What’s the best way to apply opaque gel tips?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ih93be/whats_the_best_way_to_apply_opaque_gel_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1ih935a</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Nothing fancy. Just a fun top coat (Sally Hansen unicorn TC) over black polish</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih935a</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1ih8sgv</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>just wanna share my press on with you lemme know what you think 🥰</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9av5n68un1he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1ih8jwg</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>My first attempt at gel x!</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tmx6z4il1he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1ih8gn3</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>New to nails!</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzqwreymk1he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1ih8dcp</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Couldn’t do it</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tv7n60rsj1he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1ih85bg</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>New nail style I tried today✨</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6o2uhlyph1he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1ih7wk4</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Chillin I'm my cute fur slides 👣 💅 💋 💕</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iiq5dl8jf1he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1ih7vvm</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>French tip 💅🏼</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih7vvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1ih7b3f</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Ready for valentines 💘</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ih7b3f/ready_for_valentines/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1ih77ha</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Valentine’s love bugs &amp; tea time sets</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih77ha</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1ih74x8</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>❤️</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih74x8</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1ih72ky</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>My natural nails with builder gel</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykbz4dg181he1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1ih70bk</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Autumn Color Analysis- Nude + Coral + Gold</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gr9jbp0i71he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1ih6rox</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>First time trying press-on... it didn't work well .. (or worked too well)</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tg2ivhzd51he1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1ih6peo</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Having trouble with soft gel tips</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ih6peo/having_trouble_with_soft_gel_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1ih6kna</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>how do you determine which nail shape looks best on you?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ih6kna/how_do_you_determine_which_nail_shape_looks_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1ih6k4h</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>valentine’s nails ❤️🗡️💌</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjdsd6kl31he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1ih64up</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Valentines clowns</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih64up</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1ih5tsf</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Valentines nails🖤♥️</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i9mo53aax0he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1ih5tjc</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>What can I do to make my nails grow faster and stronger?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwhc6ch8x0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1ih5rf7</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>3 hours later and a super cute set for my friend</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih5rf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1ih5mzu</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Hard Gel Question</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7go1av3ov0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1ih5mo5</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>How about this design?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kn6tgjlv0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1ih5hpk</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Valentine's Day Nails</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5d2twqfu0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1ih3quh</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Gel curing time ?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/em2oo4r4g0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1ih25xj</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>How do you extend the wear of your nail polish?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ih25xj/how_do_you_extend_the_wear_of_your_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1ih5amy</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>The Gods! 🤍</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih5amy</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1ih4hvg</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>First time trying dip nails. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih4hvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1ih594r</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Beam me up! 👽</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih594r</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1ih581e</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Scooby snacks!</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih581e</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1ih4vq0</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Kirby 💖</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih4vq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1ih4i4c</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Gel-x birthday nails ✨</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1luuo3z9m0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1ih4adp</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Opinions?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8hji7ijk0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1ih3vyb</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Saw someone post their blush/aura nails and I wanted to join</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nl6lqtoah0he1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1ih3up2</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Love is in the air!</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih3up2</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1ih3q6s</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/juagnw8zf0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1ih3pw9</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Nails needed to be done badly , so I'm ready for Valentine's Day now !</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iymyst5xf0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1ih3k9a</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>My first time doing builder gel nails</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih3k9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1ih3k5u</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>My first time doing builder gel nails</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih3k5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1ih3eiy</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Chocolates for Valentines 💝</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eo2qy4ddd0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1ih36n2</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>I think I like the red and black more</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih36n2</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1ih35ix</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>sculpted acrylic nails for my sister🎀</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0d5wgcdfb0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1ih2w88</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>more goth nails for february 🖤</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oungo3me90he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1ih2slv</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Winter icicle nails, see-through!!</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih2slv</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1ih26oj</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Purple Tweed Nails for Valentine's Day 💜</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih26oj</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1ih213y</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>💌</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqvb1vzu20he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1ih1yoj</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>How long should I rest my nails?</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ih1yoj/how_long_should_i_rest_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1ih1o7n</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>What is this yellow?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih1o7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1ih1mcl</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Fourth try at nail art!!</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ty8mr9wzzge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1ih1iy4</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Valentines set</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3zsqv28zzge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1ih1iaj</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Help with client nails lifting</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ih1iaj/help_with_client_nails_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1ih0znr</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>First proper attempt at gel polish, any tips or advice is welcome💕</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih0znr</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1igz7fn</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>How can I improve my nails’ shape?</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igz7fn</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1ih0ork</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Feedback welcome but be kind, I only completed my training course 2 weeks ago</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhiqeqh4tzge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1ih0y3q</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Loving this pink cat eye my tech did, I kinda want it all the time now! 🩷</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih0y3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1ih0n3g</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>After a lot of practice, I was able to do it</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1fvfkz0sszge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1ih0hdh</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>First Cat Eye</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p97t2f2nrzge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1igzxgd</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Light blue shimmer</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8mnsi1mnzge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1ih0c5a</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Pretty silvery blue by Dnd!</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih0c5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1ih031u</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>chrome nails with a white base</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irywiztmozge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1ih01so</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Y’all. It’s always the oval or almond option.</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ih01so/yall_its_always_the_oval_or_almond_option/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1igzlii</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>What does everyone think of acid primer?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1igzlii/what_does_everyone_think_of_acid_primer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1igzbew</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>I cant stop looking at them🌟</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igzbew</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1igz8jc</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Perfectly matched manicure</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y019o0alizge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1igz4u6</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>new fav set ✨</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eagr457zhzge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1igyzk4</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Birthday cat eye nails</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9jbgvzwgzge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1igytgw</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Valentine nails 💕</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wed5fiqfzge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1igys9t</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Written Invitation</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igys9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1igygjm</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>What nail shape suits my hands?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khxvfor4dzge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1igyc6f</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Yay or nay to the blush trend?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tsy6n6cczge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1igy952</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Last Years Sets what do you think?</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igy952</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1igxyhw</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>i should definitely start wearing rings</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7mqjacl9zge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1igxsy5</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Which shape suits me more?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igxsy5</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1igxsem</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>first set ever (july 2024) vs this week!</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igxsem</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1igxhog</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Need help! Nails are broke??</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igxhog</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1igx9kl</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Monstera nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igx9kl</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1igw31x</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>beginner gel-x</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1igw31x/beginner_gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1igw0wb</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>concert nails✨️</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y83ewmovvyge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1igvg3q</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Trying to find colours that make my hands look less…corpse-y. Mission accomplished?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igvg3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1igvawm</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Did two very different sets today!</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igvawm</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1igv5ag</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Trying my own press-ons</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igv5ag</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1igtyqr</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Here are my 3 weeks old natural Nails with only textured nail polish. Can someone recommend similar textured nail polish brands ?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igtyqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1ihcbir</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Flower glitter mani</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihcbir</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1ihbamn</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Looking for the name and brand of this color! Please help!</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nor3okn0e2he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1ihb8by</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>DripDry drops and the like?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihb8by/dripdry_drops_and_the_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1ihb6s2</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Phoenix Polish - Applejack</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihb6s2</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1ihayh9</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>$12 horseshoe mags in PPU this month!</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hmp5zdv7a2he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1ihar9e</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Best / favorite toppers?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihar9e/best_favorite_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1ihaes5</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>First, Second, and Third attempts at water marbling…there’s definitely a learning curve - stick with it!</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssl9cyc942he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1ih9jzt</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Lurid and reflective glitter: name a more iconic duo</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pfynluyfv1he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1ih8de0</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Yay or nay on these dinosaur eggs 😅</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih8de0</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1ih83oy</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Whoa baby!!</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rrnpktb9h1he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1ih7nia</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Teal With It</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qcebeyz9d1he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1ih6lsf</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Wedding Nails?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ih6lsf/wedding_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1ih61mv</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Someone is collecting people's personal information by pretending to be a buyer/seller in swap groups/subs. Be EXTRA CAREFUL whom you share your personal details with</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ih61mv/someone_is_collecting_peoples_personal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1ih5aur</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Polish ID?</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsq0bjius0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1ih5acr</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>In search for more green shades.  I would like to know your favorite 💚greens💚！</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ewvbzuzkq0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1ih5aa2</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>My first Valentine’s Day mani! ❤️💕</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1k1sywbps0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1ih50ej</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Day 3 of 14 days of Valentine’s nail inspo: Little hearts 💕</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih50ej</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1ih4a4a</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Retro Teal + Aspen</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih4a4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1ih3wn4</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Cracked nail polish</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/EyiN3qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1ih3trr</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Seche Restore</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzpia4vsg0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1ih3m6x</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Undenied by ILNP doesn’t get enough credit sometimes</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih3m6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1ih3k74</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Miss my teen years when my natural nails could grow this long by themselves</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f94yfbdme0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1ih3i1g</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Winter + Valentine’s Day Mani</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xyf6fa40e0he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1ih3eqv</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Mermaid Bait by Mooncat. Any other really shimmery colors like this you’d recommend?</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i5fh9bqed0he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1ih3eos</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Did my nails for lunar new year!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9tygqhudd0he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1ih2tl1</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>It's the little things!</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih2tl1</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1ih2sbx</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Horseshoe magnets…. Best value??</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ih2sbx/horseshoe_magnets_best_value/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1ih2mkf</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Looking for red TO black, and black TO red thermal polish</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ih2mkf/looking_for_red_to_black_and_black_to_red_thermal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1ih212v</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>I matched my new watch ❤️</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih212v</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1ih1xfi</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Best and worst thermals?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sf1otn320he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1ih1j6d</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>First Lurid Lacquer purchase, I regret not looking into this brand sooner!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih1j6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1ih18mx</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>ILNP Rosalie - I can’t decide if it looks good on me or not</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih18mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1ih0zw1</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>First skittle mani… and idk if I like it??</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih0zw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1ih0jmq</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer- Masquerade Dance Party | PPU Jan2025</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih0jmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1iguc9u</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>New nails for the next few days</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iguc9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1igxwz4</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Help with gel-x</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igxwz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1ih013d</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Cirque Lucky Bag haul</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlmc2iacozge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1igzpng</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Swamp Gloss: Fool of Misrule</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igzpng</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1igzf5m</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>v-day nails ❤️</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igzf5m</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1igzdvs</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Magnetic Velvet Effect</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igzdvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1igyrq1</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Written Invitation</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igyrq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1igyeyv</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>chihiro ✨</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igyeyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1igy66p</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Finally a red I like?!</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ndddw45bzge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1igy2qe</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Essie Apricot Cuticle Oil Grew Mold?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uu43msigazge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1igxqos</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Playing with my magnet</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g0ew1n508zge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1igxqeo</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Orly Bonder base and nail polish lifting off after 1 day</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1igxqeo/orly_bonder_base_and_nail_polish_lifting_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1igxf3x</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>ILNP - Pyro</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igxf3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1igx6ur</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Perfect Layered Glow 💜🧡💗</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igx5ob</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1igwi3e</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>How long does it take you to get through a bottle of acetone?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1igwi3e/how_long_does_it_take_you_to_get_through_a_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1igwcbh</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>My attempt at non-gel chrome!</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7p4g7a5yyge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1igvru6</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Newbie Question</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1ev5ef2uyge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1igvpe2</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Great Lakes Lacquer - A Butterfly</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igvpe2</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1igvi7o</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Trying to find colours that make my hands look less…corpse-y. Mission accomplished?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igvi7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1igvfsu</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Purples!</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4r2y49loryge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1igv3w5</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Chrome Success!</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc34dxmdpyge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1igv0qu</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Flying (US) with nail polish and nail polish remover?</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1igv0qu/flying_us_with_nail_polish_and_nail_polish_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1iguy90</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>What I asked for vs. What I got</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igqts9</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1iguwha</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Looking to match my cat's eyes</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iguwha</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1iguty3</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Cadillacquer - Many Moons 🌕✨</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iguty3</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1igu7i5</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>January manicures</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igu7i5</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1igu0n6</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Fave kbshimmer polishes?</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1igu0n6/fave_kbshimmer_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1igtik9</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Swatch Request: BKL Give Me My Agony vs. Mooncat Lord Vader</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1igtik9/swatch_request_bkl_give_me_my_agony_vs_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1igteno</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Tried a gradient for the first time. Pretty pleased with how it turned out!</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igteno</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1igt8xe</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Rogue Order Arrived!!</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igt8xe</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1igt8o5</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Such a chameleon!</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igt8o5</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1igt4xe</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Cadillaquer - What It Takes</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igt4xe</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1igs5oz</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Reflective glitter magic✨✨💖✨✨</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/84hv2qz24yge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1igrx0q</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>you know it’s a good night out when you come home looking like this</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om4npbv82yge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1igrf7o</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Its so shiny, I cannot stop staring</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igrf7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1igr7uc</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>I think Ive finally found my nude! And taken my 1st ever car nail pic</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igr7uc</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1igcmcq</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>“Root of all Evil”-mooncat</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igcmcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1igd4qp</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Penelope Luz - Purest Joy</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igd4qp</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1igf42e</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Help me find this polish!!!</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5q80nr99uge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1igqvwo</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>This is how my nails look! Any recommendations to make them grow faster?</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2swnm8l8uxge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1igqdu4</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Any advice, tips to get better</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igqdu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1igq16p</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Was the juice worth the squeeze?</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igq16p</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1igq155</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>💜⚡️Vaporwave Memphis⚡️🩵</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igq155</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1igq120</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Monday Reds</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/loh5ne53nxge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1igpgix</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>ILNP Pyro 🧨</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igpgix</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1igov21</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Mani Flashback - Valentine’s Day 2024, ILNP &amp; Zoya</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xwh8kbjvcxge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1ignywa</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>I slept on this Essie shade for way too long</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ignywa</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1igmlmz</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1igmlmz/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1igm9ox</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>I have a Fiery Attraction to EdM nail polish</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xn8a7jvbkwge1</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1ihc416</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>game art nails</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihc416</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1ihbtqm</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Ayuda!! Hice este efecto ojo de gato con gel vitral, pero no se distingue tanto. ¿Saben porque?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zo8nokr3k2he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1ihalve</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Bloom effect?</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihalve</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1ih9og0</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>My new Press Ons!</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ypc1c0qw1he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1ih8c6d</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>i never want to see a magnet again</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih8c6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1ih8bu7</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Oui Oui Baguette</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih8bu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1ih85xe</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Hand painted Valentine's Day nails!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih85xe</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1ih836q</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Ombré set 🦋</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3e4vesd6h1he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1ih67cb</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>I tried a BB belt nail!</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih67cb</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1ih5wdn</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Valentine set💕</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih5wdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1ih4018</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Snoopy nails ❤️</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ih4018</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1igz58t</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Valentines Nails! ❤️</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igz58t</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1igyxsr</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Crunchatized</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpsmsf3lgzge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1igxck4</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Valentines but make it Mickey Mouse</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mf515j95zge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1igtprp</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>My A1 client is in Japan 🇯🇵 and sent me a couple Nailfies 💅✨</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igtprp</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1igsku4</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>I finally made a tutorial on my Sakamoto nails!</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://youtu.be/MJMUO8HkLqI?si=OEPzv4z-_abzsFAq</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1igsbb6</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Pink nails I did for my birthday; hard gel top to pick crab🦀</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igsbb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1igrjs1</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>My 3rd time painting nail 🤓</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xpzx4fkfzxge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1igp17r</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Hyperfem kitty junk nails</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1igp17r</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1igo0sc</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>A special request ❤️</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8y45h8br4xge1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1iglzwb</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Hello kitty finished x</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iglzwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1iglj1q</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Are you a crystal fan?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3e2tg61qawge1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1igku7h</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Every week, I ask my 4 year old daughter some inspi for my nail art</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zodwvarb1wge1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Feb  5 08:10:52 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_09.xlsx
+++ b/data/collected_data/2025_02_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C507"/>
+  <dimension ref="A1:C700"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9052,6 +9052,3287 @@
         </is>
       </c>
     </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1ii53hr</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Wanted to make a cutesy valentine set and try out that adorable puffy heart design ❤️</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2z26r1w0ahe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1ii4nq6</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Office worker nails 🩷</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abcwd742v9he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1ii49ov</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Can't get my nails to stay on</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ii49ov/cant_get_my_nails_to_stay_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1ii34er</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Do I stay with rounded or go back to my squoval?</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usbasnukc9he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1ii2i79</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>How to distinguish a bad dip manicure from a good dip manicure?</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ii2i79/how_to_distinguish_a_bad_dip_manicure_from_a_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1ii2fuc</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Press on sets!</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii2fuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1ii1uno</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Valentines nails 💕❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii1uno</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1ii1td2</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>My Valentines Nails! Done by Naturals by Nina</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1at4ymuy8he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1ii1kvb</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Too long or just fine?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7l4z2vhw8he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1ii1jmv</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Valentines Day Nails ❤️</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sk5dz686w8he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1ii1jk7</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Loving my February nails ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mx2bzxh5w8he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1ii1htt</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>felt making a switch finally</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgjb2ezev8he1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1ii124b</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Help me troubleshoot my sister's nails</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ii124b/help_me_troubleshoot_my_sisters_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1ii18pi</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Gave my nail tech creative freedom and was not disappointed!</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii18pi</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1ii17a5</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>This thermal!!! 🍫🍓</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii17a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1ii022l</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ufzoekbi8he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1ihzs2g</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Her request was spring but with dragons, did I nail it?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihzs2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1ihyr3t</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>got nails to match an amazing pair of earrings 💖</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihyr3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1ihz6u0</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Obsessed isn't the word. 😍💅🏼😘👌🏼</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihz6u0</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1ihz0iw</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Chameleon Nails</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihz0iw</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1ihz0go</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>I’m happy :) first time getting French because my nails are so long for once and I wanted to take advantage while it lasts- I’m loving the low contrast decision</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trk3cd8598he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1ihyth1</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>No Valentine in sight this year but at least my nails look the part 😌</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihyth1</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1ihyt67</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>No Valentine in sight this year but at least my nails look the part 😌</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihyt67</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1ihxtg1</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Started painting my nails again, and I’m way out of practice. Would love any tips!</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihxtg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1ihyhuv</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>New set of claws 💅</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2s1cqwn48he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1ihycv7</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Red cat eye hearts for v day ♥️</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9p6viv6g38he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1ihy17b</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Valentine’s Nails🩷</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7usm4z7m08he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1ihy0uo</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>I wear my heart on my nails ♥️</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xm8g4sxj08he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1ihxswv</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>New green set</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihxswv</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1ihxrpg</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Feeling girly and glam with these pink pretties! 💖</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihxrpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1ihxhk3</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihxhk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1ihxe08</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Wedding nails!</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihxe08</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1ihx48e</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Cat eye butterflies 💜🦋</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihx48e</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1ihx4dp</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>I did my own nails 💅 and I love them</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hnm5tymzs7he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1ihx1zs</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cp2tgv9gs7he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1ihwfrp</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>What e file bits do you use for flawless cuticles?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihwfrp/what_e_file_bits_do_you_use_for_flawless_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1ihw9pr</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Sakura as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihw9pr</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1ihw7ni</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>In appropriate conversation hearts</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73dkmthel7he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1ihvwen</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Snake Nails</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihvwen</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1ihvupk</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Lunar New Year Nails</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihvupk</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1ihvmwx</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>So shiny, so chrome</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fl7ym04rg7he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1ihvec5</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>valentine nails❤️</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83m6cseue7he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1ihv995</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>15 yr old niece’s creation</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihv995</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1ihuas6</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Birthday Mushie Nails</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihuas6</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1ihucm7</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Week old DIY dip... I'm wondering if it's safe to file and shape the nails more into almond then do another dip, activator and top coat, or if I should just leave it</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5nahaeu67he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1ihucav</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Valentines nails 💋💕</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/olys3b6s67he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1ihubo9</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Does a High-Quality UV Base Gel Prevent Chemical Exposure from Colour Gel?</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihubo9/does_a_highquality_uv_base_gel_prevent_chemical/</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1ihtf5i</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Is this normal from a gel manicure?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihtf5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1ihtn28</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>when did nail salons get so freaking expensive?!</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihtn28/when_did_nail_salons_get_so_freaking_expensive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1ihtzti</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>First time kinda</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inclur5647he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1ihu2k9</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Hand-drawn stained glass roses that my tech absolutely CRUSHED 🌹</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kkkik0nq47he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1ihtyzu</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Long square white nails</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihtyzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1ihtm90</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Blue nails</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihtm90</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1ihtf8m</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>A little Valentine’s Day love ❤️</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihtf8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1ihsym2</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Am i wrong nail techs?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihsym2/am_i_wrong_nail_techs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1ihspen</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>First time ever doing oval...</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihspen</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1ihslwf</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>strawberry set 🍓</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihslwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1ihsl0m</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Celestial set</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihsl0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1ihskt3</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Am I crazy for expecting literal perfection when i pay to get my nails done? I mean, I find them pretty, but still see some imperfections in the shape...</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihskt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1ihs9y7</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Hair getting caught in nail charms</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihs9y7/hair_getting_caught_in_nail_charms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1ihs1rq</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>My first time doing designs</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihs1rq</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1ihrlhq</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Kids got into superglue and used it to put on press on nails, anyway to remove them?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihrlhq/kids_got_into_superglue_and_used_it_to_put_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1ihrjuh</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>What do you guys think ??</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dnm9p5bm6he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1ihrf5h</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Simple Valentine's Nails ❣️</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6m5va5vcl6he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1ihrcwj</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Did I get scammed?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlha74hwk6he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1ihqd06</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Discontinued press ons</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arlwe5xod6he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1ihqiie</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Please help me &amp; be nice or I’ll cry</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihqiie</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1ihqmci</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Fresh set!</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkcrz1elf6he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1ihqkc3</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Semipermanent pink with animal print</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihqkc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1ihqafe</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Practicing gel on fake hand 💅</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0dvcyh5d6he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1ihq58h</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Currently started on making my first set!!! 😁 🎉 💅</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqdjca93c6he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1ihpnod</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>LONG NAILS - what are we doing?</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihpnod/long_nails_what_are_we_doing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1ihpnww</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Soft gel 🫶🏻😍</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtag8tom86he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1ihonyp</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>February set :)</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihonyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1ihpb31</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>V-day ♥️</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lltk0t066he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1ihozra</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>um my friend sent me this</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihozra</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1ihozm3</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Valentines Candy Hearts Set 🥰</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6reqd5vm36he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1ihozgv</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Valentines Day Nails?</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihozgv/valentines_day_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1ihox9o</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Some press one I’ve made recently!</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihox9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1ihoil8</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Suggestions please</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vs0lc1yb06he1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1ihhqgd</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Why do my nails do this?</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihhqgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1iho9pi</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>I'm happy with it pink colour</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wx7qqp7ly5he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1iho6r9</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Is this normal practice?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iho6r9/is_this_normal_practice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1iho2zf</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Little bit of Valentines vibes</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bvaqdz7x5he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1iho07d</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Awww 🥹 what do you think about my new work?</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iho07d</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1ihnx22</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Valentines set w/ a twist</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfvt7k43w5he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1ihnvql</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>I would like to get my nails done but I am not sure what I should get.</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihnvql/i_would_like_to_get_my_nails_done_but_i_am_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1ihnjxh</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Purple french tips</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5qf0kggt5he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1ihmzwq</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Can the cat eye nail trend be done on natural nails? Or is it gel only?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihmzwq/can_the_cat_eye_nail_trend_be_done_on_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1ihn6tz</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Nail newbie help</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihn6tz/nail_newbie_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1ihmslx</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>New Set 🥰</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihmslx</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1ihhkef</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Why can't I wear nail polish or fake nails?</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihhkef/why_cant_i_wear_nail_polish_or_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1ihe9d6</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Acrylic nails lift/fall off after a week?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ihe9d6/acrylic_nails_liftfall_off_after_a_week/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1ihjg14</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>I didn’t apply my press ons correctly and now my nails look terrible, what can I do to heal them?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uo9rx0wwy4he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1ihjs8b</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Valentine’s Day inspired nails 💓❤️</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssc8etlk15he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1ihma0d</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>My nails today❤️</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6x7u929k5he1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1ihm8jh</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Birthday nails!!!</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihm8jh</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1ihltl2</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>My bday set!</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bpl4ueyg5he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1ihlqsu</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>colour recommends</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihlqsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1ihlnza</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>My first Valentine’s set 💕</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihlnza</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1ii56e4</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Ready for Valentine's ❤️</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/be320tyz1ahe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1ii52lt</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Torn</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wpkaz0l0ahe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1ii4ixz</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>After 2 days of wear!</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii4ixz</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1ii48ga</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Please tell me the “out of stock” on Polish Pickup is just a placeholder 😭</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ii48ga/please_tell_me_the_out_of_stock_on_polish_pickup/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1ii3ycy</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>What are cuticles supposed to look like?</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngsimki6m9he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1ii2bg2</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>My first attempt at using tips and rubber gel</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmgjodgz39he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1ii1bh9</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Can't decide if I love or hate these...</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii1bh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1ii1ans</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>I’m in LOVE with my latest mani! It took me HOURS.. but it was worth it</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii1ans</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1ii12ua</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Funeral Home Polishes</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ii12ua/funeral_home_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1ii0xqx</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Orange with green shimmer?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ii0xqx/orange_with_green_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1ii0ud9</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>ILNP Spiced Cider</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/40h891rfp8he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1ii03f7</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Go Birds!</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii03f7</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1ihzw3h</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Possible dupe for Jewel of the Ball?</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihzw3h/possible_dupe_for_jewel_of_the_ball/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1ihzbos</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Orly's spring 2025 ad - girl you know I love a 70s theme but does this not look like salad dressing??</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihzbos</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1ihz8mm</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Accidentally matched my PJs 😴</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jlvsaeb1b8he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1ihyrps</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Starrily yanked my wig to the side a little with this jelly 😍</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihyrps</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1ihyk91</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>I mixed my own jelly jade polish, then realized it matched my fancy teacup :)</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3rc0mav858he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1ihybtr</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>brands that sell solar/UV nail polish?</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihybtr/brands_that_sell_solaruv_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1ihy189</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>moody shimmer</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihy189</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1ihx7f0</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Question re: horseshoe magnets 🧲</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihx7f0/question_re_horseshoe_magnets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1ihwvef</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Mooncat Jewel Beetle is distracting.</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5spojlwq7he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1ihwnbh</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>I filmed using the alcohol inks in my sally Hansen jellies</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://youtu.be/QjE9zXLxmvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1ihwgkl</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Clean-up Brush for shimmer particles?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihwgkl/cleanup_brush_for_shimmer_particles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1ihwgdr</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>First time trying ILNP</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihwgdr</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1ihw1dj</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Mushroom Nails</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihw1dj</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1ihvmcz</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Nail polish vs. Lacquer?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihvmcz/nail_polish_vs_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1ihvlgq</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>first time trying hearts</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihvlgq</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1ihv0ak</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>“Classic” Red  still not sure about the shape but over all am happy with the end result!</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihv0ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1ihux1f</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>first time putting a jelly glitter over a crème!</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihux1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1ihutpv</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>First Clionadh Order</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1biznl9ga7he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1ihuh4l</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>BKL [redacted] ID?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihuh4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1ihudjh</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Pls help me ID nail color</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihudjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1ihtb5g</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Non usa brands</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihtb5g/non_usa_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1iht3bg</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>This one sparks joy 🌟</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iht3bg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1ihsm1w</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>L.A Colors Nova</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihsm1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1ihsgv6</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Day 4 of 14 days of Valentine’s nail inspo! Star studded ⭐️</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihsgv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1ihsfbg</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Iridescent 💜🩵</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihsfbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1ihs3h9</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Simple butterfly nails 🦋</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihs3h9</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1ihrn1y</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Tried to stay on theme with the choices...</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gk9wy3aym6he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1ihrazs</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>I present to you, my first Sassy Sauce haul!</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihrazs</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1ihqo1b</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>You can tell when I stopped using ORLY Bonder due to the damage it was causing</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utsbfotxf6he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1ihqj2c</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Something clean and simple</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihqj2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1ihq9ie</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Happy Anniversary to The Sims 4</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1fafx5uyc6he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1ihq4kb</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Cirque Colors Catalina - 3 coats, 11 days, and one twin birth later</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihq4kb</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1ihpxrb</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>What are some good fast-drying top coats?</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihpxrb/what_are_some_good_fastdrying_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1ihptu1</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>It's Giving Mardi Gras 🎉🎭</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihptu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1ihpo89</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>More love for Bill!</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l7vhlt6n86he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1ihpgb7</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Had fun with some layering!</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihpgb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1ihohnu</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>A loud AF nail girly looking for neutrals that won’t bore me. Drop ur recs!</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krc2scx506he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1ihocqp</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Team Green is GOOOOOOOOOO! 💚🦎</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihocqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1iho7tv</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>MCR Nail Art</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iho7tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1ihnw1h</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Took a while but was worth it🎀</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hcncixtv5he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1ihmvsm</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Dupe for Lilypad Lacquer's Iguana Be Wild?</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/192h4kvjo5he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1ihmik1</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Lumen Starfall Ball 🌟</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihmik1</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1ihlpxs</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Looking for dupe!</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihlpxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1ihlgob</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Possible jellies spotted at Dollar Tree</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihlgob</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1ihlagq</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Switching from natural nails to press ons, need some help</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihlagq/switching_from_natural_nails_to_press_ons_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1ihl4yv</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Valentines Day 2025 Mani: ILNP + Psyche Minerals - thoughts?</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihl4yv</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1ihkzcg</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>January update for my 2025 mani tracker blanket</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihkzcg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1ihkgam</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>pretty in pink 🩷</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihkgam</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1ihjica</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>ILNP Eclipse - I finally get the hype</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihjica</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1ihjhb0</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>ILNP Evermore in the sunlight is everything 💕💕💕</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/841es6i7z4he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1ihjc3c</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>You guys are a bad influence!</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2kivtqzx4he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1ihivb5</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>🏺🌟Kintsugi🌟🏺</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihivb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1ihhvuo</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Not sure how I feel about this color but the magnetic sure is beautiful</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ldjob4srl4he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1ihh701</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>First magnetic polish swatch</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihh701/first_magnetic_polish_swatch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1ihgrfe</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Should I go matte for this box of chocolates? 🍫</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihgrfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1ih7rlx</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Superbowl ready!</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f00hqau8e1he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1ihedmm</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>How to decide on a polish in-person?</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihedmm/how_to_decide_on_a_polish_inperson/</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1ihduzs</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Sea-ing Is Believing</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihduzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1ihdr99</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>are there any press ons that you can take off whenever?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihdr99/are_there_any_press_ons_that_you_can_take_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1ii557i</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>4th wing nails done by me (licensed)</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii557i</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1ii538w</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Aquarium Valentine Set 🥰</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pyhgalt0ahe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1ii17vx</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>practicing my nail art day by day🥰</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2jv9s20t8he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1ii3i24</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Once upon a broken heart Valentine’s Day nails 🫶 by me 💅</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii3i24</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1ii21rq</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Valentine's Day Nail Sets</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii21rq</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1ii20lx</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>This one’s for My Latinas ✨🌹</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1d8vznx09he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1ii1rkv</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>I finally did the magnetic French tip!</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3t67vy0cy8he1</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1ii1osb</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>My Valentines nails!</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkemn7ekx8he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1ii1myy</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Valentines nails!</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii1myy</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1ii0wlm</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>V-Day Nails!!</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5e9iti2q8he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1ii0uds</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Orange Checker + Wine</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g32mayjhp8he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1ihxe5w</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Valentine look #2 which one do you guys like better this or my previous post?</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihxe5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1ihwab6</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Sakura as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihwab6</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1ihvusw</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Snake Nails</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihvusw</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1ihtn4w</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Vday nails, whatcha think?</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihtn4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1ihsixo</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Celestial set</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihsixo</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1ihpr89</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Corny birthday present for a friend</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/comyg3pa96he1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1ihme77</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Winnie the Pooh nail set</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ihme77</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1ihkvan</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Valentine set ❤️</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xju16mqx95he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1ihitd0</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Happy lunar new year 🐍🏮✨</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxlfytrrt4he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1ihdjvc</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Making my vision a reality for my clients 💞</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhhb4ttj73he1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1ihdcsr</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Simple valentines set for my mami</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6bxcfju43he1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Feb  6 08:11:01 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_09.xlsx
+++ b/data/collected_data/2025_02_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C700"/>
+  <dimension ref="A1:C880"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12333,6 +12333,3066 @@
         </is>
       </c>
     </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1iiwsvz</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>help!!!!</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqu6pp65xghe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1iiqx90</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Appointment in a few days. Dunno what to do (natural nail, builder gel)</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiqx90</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1iiumru</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Which one is better: UV gel or glue?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiumru</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1iitrj6</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Onycholysis</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iitrj6/onycholysis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1iiw13i</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Finally decided to do my Valentine’s Day nails, I like how they turned out 🥰🥰</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odcvcbysnghe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1iivnzn</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>My Valentine's Nails</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iivnzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1iivm5b</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Bath time and Barbie nails</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ky729lh1jghe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1iivjh0</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>I love my hands full of colors</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jv7eb1n6ighe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1iiuuvx</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>my second manicure on natural nails!</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/730vbecxaghe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1iiukhv</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Kirby Valentine’s Day nails!</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiukhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1iiu68s</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>more nails I got done in the past years…</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiu68s</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1iitd4l</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>A little derpy but getting better!!</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iitd4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1iitccv</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>How to stop nail polish from chipping?</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iitccv/how_to_stop_nail_polish_from_chipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1iissaj</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Valentine's Day nails</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uddltr1rqfhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1iismw8</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>did my own nails and used charms for the first time 🌸</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iismw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1iiretj</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Is this onycholysis?</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1anutfndefhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1iirzyp</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Valentine’s Day ready. 💅🏼💋💘</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xz8pixkjfhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1iiry8k</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>My nails are more organized than my life. 😅</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekyf9wb2jfhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1iiroo8</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>My third nail design and my favorite so far so I wanna share</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/397lyv9rgfhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1iir6nv</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Press ons that don’t stay very long?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iir6nv/press_ons_that_dont_stay_very_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1iiql7q</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Vday Set!</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kki5srn37fhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1iiqgxg</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Thanks, I hate it.</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4i7df7g36fhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1iiqagz</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>I need help</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiqagz</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1iiq8xc</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Dazzle Dry or Nailboo?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9b5mz3864fhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1iiq7bs</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>My Melody Nails</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiq7bs</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1iiq475</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Sugar ..Spice and Everything Nice.</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5a7qw7433fhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1iipz54</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>My Valentine’s nails 🖤</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iipz54</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1iiptkk</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>What do you think of this rich brown shade? Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiptkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1iiprtv</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>I really like this shade of Red</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xla6het60fhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1iipiqz</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Whenever I push back my cuticles, they start looking crusty.</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iipiqz/whenever_i_push_back_my_cuticles_they_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1iiph34</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Clean French with pearl chrome</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiph34</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1iipfik</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Guys am i crazy or what!!!!!!!!!!!!!!!! So i was doing my polygel nail and then i realize my slip solution was finish u know what i use and it work really well PERFUME!!!!!!!!!!!!!!!!!!!!</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iipfik/guys_am_i_crazy_or_what_so_i_was_doing_my_polygel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1iioxjz</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Favourite cuticle care?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iioxjz/favourite_cuticle_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1iioops</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>My take on fishing lure nails!</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6l4fpcf4rehe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1iiofui</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Bridal nails</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiofui</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1iio5s1</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>To whoever I saw on here suggesting a rubber base coat….</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iio5s1/to_whoever_i_saw_on_here_suggesting_a_rubber_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1iio3ky</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Chop or extend, help please!</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iio3ky</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1iinigf</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>What was the best nail advice you’ve ever gotten?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iinigf/what_was_the_best_nail_advice_youve_ever_gotten/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1iimp13</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Little bit of Green before the Superbowl. Go Birds!!🦅</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84qr5m3mbehe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1iimg6g</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>What type of nails are best to make for a beginner?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iimg6g/what_type_of_nails_are_best_to_make_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1iimf0f</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Suggestions for color changing kid safe polish?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iimf0f/suggestions_for_color_changing_kid_safe_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1iimdm9</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Birthday nails 💅🏾</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkaqjeo99ehe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1iimbrg</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Getting ready for Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vwipilt8ehe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1iilxwn</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Such a warm color, what do you think?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hw8fnd106ehe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1iiln1c</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Why do my nails always crease?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiln1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1iilvp2</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Siri, play Bite Size by SixSaidIt</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iilvp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1iikrvh</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>My New Set for the month of February/Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iikrvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1iil3rm</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails activated 💅💜💕</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddu7dhiqzdhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1iil2l4</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Do you like the shape of my nails?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxfkejhkzdhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1iikmth</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>They absolutely destroyed my nails and I’m a bridesmaids at my friend wedding in 1 week…</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iikmth</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1iikec0</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Did someone try this? is it comfortable?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4afdyuwqudhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1iik9xx</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>DIY leopard spots to match my hair :)</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fuodwvrttdhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1iik4fh</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Hyper realistic nails</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iik4fh/hyper_realistic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1iijxph</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>forgot post this press on set I made for my bestie for christmas 🍊🐬🌸</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ul1c8vpbrdhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1iijvqr</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>New New!</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ch2u80zwqdhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1iijqam</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>CUTE PRESS ON’S TILL THE DAY I DIE!!!!</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iijqam</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1iijbek</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Strawberries 🍓 dipped in chocolate 🍫</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8onmrwasmdhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1iij613</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Just did these valentine nails this morning ❤️</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://imgur.com/pCQx5cB</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1iij3kq</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Corrin(s) &amp; Siblings Full Nail Set!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iij3kq</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1iiizdf</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>My gf does nails on the side and I keep telling her she’s pro level. Love these so much! 💕</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiizdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1iihta7</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>ready for valentines!</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y88f9v0cdhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1ii72hg</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Help i broke my nail… (don’t swipe on photos unless you’re ok with seeing nail damage)</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii72hg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1iiiqr9</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2y84xoepidhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1iiio5n</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Love me an extra girl🐅🐆🧡</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiio5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1iiihq9</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Post soak off</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irjvqvuugdhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1iii8nn</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>BCB Lacquers - Tears of the Kingdom 🗡️</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iii8nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1iihwvm</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>I made my own press-ons!</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iihwvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1iihut9</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Valentine Frenchies 💖</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pz1v2j1ccdhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1iihtq3</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Cat eye butterflies 💜🦋</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iihtq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1iihdla</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cl7j7mx8dhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1iih6fa</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Nails are completely damaged</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iih6fa/nails_are_completely_damaged/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1iih5qs</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Which brand of press-ons don’t do THIS ? (Nails Break In Half)</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3r6so0d7dhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1iih2vy</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>I don't always try glitter, but here goes</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frwgyt5t6dhe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1iih1yy</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Hawaii nails</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iih1yy</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1iih1re</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Hawaii nails</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iih1re</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1iigwyr</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>late lunar new year’s set!</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iigwyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1iigp4q</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>I’m obsessed! Aren’t you?</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1q8v2re04dhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1iige18</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Lipstick Press Ons</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llvf6o8s1dhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1iig7gp</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Got my nails done for Valentines and Galentines days</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jff2ok8i0dhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1iig2o6</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Anyone else do 2 sets of valentines nails ???</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iig2o6</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1iifxkg</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Look familiar?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyxlz7igyche1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1iifoyy</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>A little heart design I made today</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iifoyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1iif96l</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>At home set ups</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iif96l/at_home_set_ups/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1iibg1d</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Love my nails but suddenly allergic to UV? Used to do SNS But my nails were getting very brittle. Would press-ons be an option?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpvb5lwb1che1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1ii6wzw</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Poly gel set recommendations</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ii6wzw/poly_gel_set_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1ii6l1m</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>I cut my skin and it bleed, can i still proceed…</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ii6l1m/i_cut_my_skin_and_it_bleed_can_i_still_proceed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1ii7os8</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>What happened to my poor nails :/</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/at7g2sf70bhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1iieyj6</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Red with a heart ❤️</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iieyj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1ii8v7k</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>hema free base/glue for extensions</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ii8v7k/hema_free_baseglue_for_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1iieq13</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Short nails can be fun too ✨</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iieq13</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1iiemv0</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Valentine’s Day!</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiemv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1iiejlq</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiejlq</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1iiebkh</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Obsessed with this design</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwff1sttmche1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1iidz46</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>I’m obssessed with my new nails</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5h4wtmuakche1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1iidnnm</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Valentines Day Hypno Nails</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iidnnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1iidhit</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Want to do my nat nails myself, never did before, please drop suggestions</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qm7uk1trgche1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1iid81e</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>my dog was diagnosed with cancer. so I got a set just for her.</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iid81e</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1iid01l</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Former Nail Biter</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iid01l</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1iicyvy</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Throwback one week ago to my birthday set</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2gjgohj0dche1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1iicem9</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Will gel never work for me?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iicem9/will_gel_never_work_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1iix6k8</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Help, please. ISO a really good red-orange polish.</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/la0l1hf42hhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1iix6cn</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Owl Bear Cub BKL vs Dark Horse MC</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iix6cn/owl_bear_cub_bkl_vs_dark_horse_mc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1iivs2x</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>What color is this? Help!</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iivs2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1iivmai</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Death Valley Nails - Curiousity Cloud</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzt24q33jghe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1iivb4n</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Can someone help me find a nail lacquer like this? No gel please</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vp1vb1ifghe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1iiu5od</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>multichrome love 🥰</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n9rfz32b3ghe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1iitvyi</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>What I got in my Cirque Colors Lucky Bag</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iitvyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1iit69n</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Day 5 Fool's Paradise</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnmk38qfufhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1iisqu3</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Go Birds</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iisqu3</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1iirqvo</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Give me your rainbows!🌈</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iirqvo/give_me_your_rainbows/</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1iirgrj</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>OG Sally Hansen’s PACIFIC BLUE 💙</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iirgrj</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1iir2je</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Why chose one purple when I can a skittle of them on my hand?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iir2je</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1iir2df</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Polishes with Monster Energy Vibes?</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iir2df</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1iiq1pv</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Same, same but different ✨️🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiq1pv</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1iipoxo</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Whenever I have a broken nail I always think it looks like a little bald guy.</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cx02xo8hzehe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1iip2w3</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>please someone tell me these are similar enough and that i don’t need both 😵‍💫  i already own cat’s paw.</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iip2w3</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1iioly4</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>my first thermal 🖤</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/efcw1fjhqehe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1iiod9q</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>♥️✨Too much Balatro✨💙</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiod9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1iinpt3</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Discovered an interesting warm-to-cool shift!</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iinpt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1iimuj5</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Illusionist</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iimuj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1iimo25</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Fanta-Sea by Apres</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34hcbw1fbehe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1iilm4l</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>ILNP vs Mooncat wwyd?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iilm4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1iilfkb</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Anyone know a dupe for Lurid Lacquer’s “Tibberz!!”?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lov2cqo72ehe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1iil972</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>First time with stickers!</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1rujhix0ehe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1iiktpt</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>What about this Blue?</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiktpt</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1iikt41</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>What about this Blue?</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iikt41</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1iikn5q</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Valentine Mani</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rw6e4nwjwdhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1iik477</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Base Coat Battle Bracket</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iik477</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1iik2p2</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Ethereal - Enchant Me</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iik2p2</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1iiiz3w</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Swatches of your fave magnetic toppers?  🧲⬆</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iiiz3w/swatches_of_your_fave_magnetic_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1iiinli</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>My first glow in the dark polish is a ✨stunner✨! Colores de Carol - “Love Is… A Little Cheesy”</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiinli</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1iiigot</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>🩷 BCB Lacquers Back Shot 🤍</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiigot</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1iii9jv</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>BCB Lacquers - Tears of the Kingdom 🗡️</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iii9jv</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1iii99w</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>sometimes shorties are the way to go 🍬</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/foy80xv5fdhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1iihdkx</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Chinese Press On "Glue" and HEMA</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iihdkx/chinese_press_on_glue_and_hema/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1iigwrl</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Update: Found the full L.A. Colors display with jellies and more at the Dollar Tree!</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ith90wkk5dhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1iigvwb</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Clionadh - sales?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iigvwb/clionadh_sales/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1iignfc</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>LA Colors - rave review for $1 polish</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iignfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1iigkie</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>You guys!  I shaped my nails!  Also, this color…🤩</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iigkie</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1iig4ha</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Holo Skittle 💜💕</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iig4ha</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1iifzey</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Palate cleanser</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yolyvwvyche1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1iifwjg</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>💖💋Hot To Go⭐️🗽</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iifwjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1iifu9d</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Overdrive is offensively sheer. Ended up doing 4 not-so-thin coats. Used a QDTC and still smudged two nails 2 hours later</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a544ki92xche1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1iifpg2</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Nail vinyl recommendations?</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yh99ilvwche1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1iifafj</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Fierce Mojo is INSANE</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ssgbnybrtche1</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1iif759</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>HELP ISO</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iif759</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1iiewtk</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Mixed feelings about this polish.</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ulz1ziq2rche1</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1iiek7g</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>I need a detective! Can you find me a metallic medium particle yellow-orange shift</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iiek7g/i_need_a_detective_can_you_find_me_a_metallic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1iiefn3</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Veil of Illusion by Beaux-Reve and Mourir d’Amour by Femme Fatale</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiefn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1iidmkx</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>When magnetics are totally worth the extra work</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iidmkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1iidchc</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Maelstrom: yea or nay?</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v44rcsasfche1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1iicssp</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>RedditLaqueristas inspired purchase ❤️</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iicssp</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1iichgz</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Quest to find the perfect blurple</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iichgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1iibnnn</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Perfect Love</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iibnnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1iibdxp</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>More of this!!</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii0pv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1iia8yq</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Man I love mooncats polishes but...</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofbplvmirbhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1iia7oo</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>What will make my nails look like a disco ball?</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iia7oo/what_will_make_my_nails_look_like_a_disco_ball/</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1ii95bb</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Mooncat Fields of Lavender</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii95bb</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1ii7qnw</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>This is not a peel off base coat :(</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hacurjat0bhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1ihryg4</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>How to not chew off nails</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ihryg4/how_to_not_chew_off_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1ii0vmo</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Low maintenance clean nail polish</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ii0vmo/low_maintenance_clean_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1ii1z1z</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Sculpted Hearts Valentines Set  🥰- Gel and Laquer Combo</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii1z1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1ii5z1r</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Ready for Sunday!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ii5z1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1ii5kud</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>January nails</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1oo7i9c7ahe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1iiuk3v</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>My first chrome effect nails</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ynz4rmw7ghe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1iiqtps</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>did my friends bday nails!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqp638869fhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1iiqp0c</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Did my nails</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiqp0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1iiqhwj</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>AOT SET</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am7kmqgb6fhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1iiod9k</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Chrome Hearts Valentines Day Nails</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiod9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1iinc3g</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Nails by my friend 🙏🙏😍</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9o90wxfggehe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1iij4yx</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Corrin(s) &amp; Siblings Full Nail Set!</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iij4yx</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1iiikac</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>My sibling is wanting to get into nail art, so I want to get a gift: What nail art kits are Good?</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1iiikac/my_sibling_is_wanting_to_get_into_nail_art_so_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1iii6ca</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Nail Art Beginner</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1iii6ca/nail_art_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1iih0mf</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>late lunar new year set!</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iih0mf</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1iigxwr</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>I feel so much happier when my nails look this fine 😍</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3yel1dws5dhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1iigd7m</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>2nd time wearing this set🥰</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iigd7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1iidfl5</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Custom ordered press on set 🐆 🍒 🌺</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iidfl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1iid5tm</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>stich nails🐾✨</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltyop4lheche1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1iibv5f</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Planning on wearing these to my sister's divorce party</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iibv5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1iibh2m</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Frutiger areo, probably one the the best set I done since i started to do my nails last month</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iibh2m</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Feb  7 08:10:47 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_09.xlsx
+++ b/data/collected_data/2025_02_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C880"/>
+  <dimension ref="A1:C1088"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15393,6 +15393,3542 @@
         </is>
       </c>
     </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1ijq227</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Lunar New Year/ Valentine's Nails ❤️</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fd9otuhicohe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1ijpgtn</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Got new nails yesterday and not a fan of them</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ijpgtn/got_new_nails_yesterday_and_not_a_fan_of_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1ijp694</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Blue flower vacation nails for my client 🤭 LOVEE how they turned out, But I know I can make improvements</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ojp66et0ohe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1ijozup</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>lips valentines nails</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijozup</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1ijot57</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Polygel lazy girl method + method. For once, I'm happy with my application :P</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijot57</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1ijot1w</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Reddddd</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e52dhcd8wnhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1ijoo21</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Red for Valentine’s Day ♥️</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijoo21</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1ijomhk</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>I can't find anyone that has nails that look or act like mine. More info in comment.</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a49hmtx1unhe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1ijofv9</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>When your nails match the season and the holiday and of course your outfit. Cold Af out so Black ice and zombie valentine.</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51l8ln8yrnhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1ijnc7k</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>What do I book?  Pic Credit: Ava Lane &amp; Co Pinterest</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwyfcecxfnhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1ijo2jg</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>lowkey Vday nails</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijo2jg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1ijo26f</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>lowkey Vday nails</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijo26f</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1ijnyqo</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Valentine set</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijnyqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1ijnthd</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Tip of the Day!!!!! Learn from my mistake.</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egp8c291lnhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1ijneli</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Ideas to match the dress</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rogvdqcmgnhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1ijn1gy</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Freehand Tarot Nails🤍</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jabho3awcnhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1ijmwe4</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Subtle Valentine's Day Nails (with new wedding band!)</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijmwe4</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1ijkxm4</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Looking for inspiration…</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ijkxm4/looking_for_inspiration/</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1ijmuat</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Re-created a photo I saw on Pinterest 💅🏽</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkf50buuanhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1ijkov7</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>My take on the tiktok valentines nail trend</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epywv9t9qmhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1ijlrsv</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Which one is better: UV gel or regular nail glue?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ijlrsv/which_one_is_better_uv_gel_or_regular_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1ijmaqd</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>What in the crackle?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ehu621e5nhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1ijmd4z</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>What I got vs what I asked for - inspo from @Vettsystore on IG</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijmd4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1ijmosm</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>European manicure</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ijmosm/european_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1ijmg7f</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>This is the first time I've been able to grow my nails out this long. I'm going to a manicure but tbh I'm not sure what shape would fit me best. Could you please help me ?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijmg7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1ijm9l0</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Cat eye nails for Valentine's Day ❤️🖤</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijm9l0</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1ijm7i4</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>rose quartz nails</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijm7i4</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1ijlz6p</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>First Time Using Builder Gel</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijlz6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1ijleg3</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>my gloomy nails for this gloomy weather 🌧️</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijleg3</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1ijkccm</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Valentines Day Nails</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/syrcsc62nmhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1ijjj83</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Help!!</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ijjj83/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1ijgo2h</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Does anyone know a way to fix my nail from bending like this?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89sjrk0arlhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1ijh8a5</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>I can’t seem to figure out sizing on nail tips.</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijh8a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1ijk2ic</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>My birthday set</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijk2ic</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1ijjyi2</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Best friend of 16yrs my loves, and one who tries to out do my nails. 🏳️‍🌈👨‍❤️‍👨💅</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11hcgyekjmhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1ijjyan</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Valentine Nails 💅🏼 🩷💕</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijjyan</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1ijjwyu</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Tired of nails peeling</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ijjwyu/tired_of_nails_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1ijjtee</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>What are “fills”? How many times can you do them before you have to get a full set again ?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ijjtee/what_are_fills_how_many_times_can_you_do_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1ijjp1e</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Not long ago, I wrote about how one nail technician ruined my nails.</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijjp1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1ijjoqn</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Ladybug nails 🐞</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijjoqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1ijjmpw</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Mermaid vibes only 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijjmpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ijjl0h</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Can I bring this dip powder to nail salon?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://a.co/d/dy1JxQR</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1ijiyt8</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>New set for Feb 🍒 ♥️</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1xcvdqpamhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1ijiv4f</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Length and Strength</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ijiv4f/length_and_strength/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1ijiu0r</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Checkmate</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9x246ej9mhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1ijim0s</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Valentine's Day press ons I made myself 💌🎀</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/croh7j6m7mhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1ijhzol</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Gel x</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fr4iotk62mhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1ijhw9e</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>what nail shape would suit my hands?</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijhw9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1ijhl1d</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>First time trying a cateye french (plus chrome to hide the fact it’s very obviously a first attempt)</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5jdvik3qylhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1ijhj00</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>What do we think about the color and shape here?</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijhj00</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1ijhb77</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>I just got this beautiful matte set but I’m slightly regretting the finish. Advice needed!</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zo0z9ijkwlhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1ijh7sw</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>❤️🩷❤️🩷</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02mhk9lrvlhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1ijh5gq</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>How did they turn out? I made them for my mother 🥰</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvr8h4i7vlhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1ijgzxx</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>February Nails🎀💌❣️💗</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7b0aeznwtlhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1ijgs4c</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>🥰🥰</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0cutl5n5slhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1ijge7x</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>i’m a beginner nail tech and haven’t been really motivated to do nails but yesterday i did a short set for the first time ! (i usually do them really long lol ) any way to improve ?</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijge7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1ijg002</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>My and my husband’s wedding nails</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpt7qxv1mlhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1ijfukp</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Valentine's Day 💘💌</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emev4ebwklhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1ijf3jj</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Ointment</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijf3jj</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1ijernw</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>valentine’s day nails!! (press ons with nail glue from Sally’s!) 💕</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrd6s83pclhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1ijerlw</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>How to use these charms?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijerlw</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1ijepgl</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Is this fast growth?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijepgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1ijee2c</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>How do you get nail polish off of skin?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ijee2c/how_do_you_get_nail_polish_off_of_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1ije4gm</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>A collection of some of my BIAB nail art (spot the odd one out 😅)</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ije4gm</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1ijdqm1</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Valentines is approaching!</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1fuwz6375lhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1ijdp8d</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>I keep wanting to like this color but…</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b607iydx4lhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1ijdcdc</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Ready for Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pmlpplc2lhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1ijd9p9</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Product suggestions?</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijd9p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1ijd1nt</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Late to the plastic wrap trend</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ehx9y190lhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1ijch65</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Can someone recommend a physical store to buy chrome powder in Melbourne?</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ijch65/can_someone_recommend_a_physical_store_to_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1ijctcs</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>On theme for the month</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5yjpynjykhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1ijcp4x</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>💕</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkjeavgoxkhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1ijclqd</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Nail glue</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usmyakdzwkhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1ijc5ek</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Fresh Mani Love</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ppyopb3otkhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1ijamps</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Very first time doing gel nails myself!</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sraaf71oikhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1ijbl8g</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Is it possible my pedicurist is doing this on purpose?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep4amofqpkhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1ijbetx</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>these are press ons 🤍🌺🪻</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijbetx</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1ijax53</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>recent set:3</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijax53</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1ijars6</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Pretty in Pink</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asdb9sznjkhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1ijalzg</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>My lilac fingers from January🪻💜</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47o9dzqiikhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1ija3o2</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Should I start learning to be a nail tech?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ija3o2/should_i_start_learning_to_be_a_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1ija0rr</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Another set of press ons!</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ija0rr</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1ij9jro</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Does this shade of red suit my skin tone?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij9jro</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1ij9h58</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Beginner - Custom Press-On Nails 💅✨ (Help Needed!)</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mc248lucakhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1iion1k</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iion1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1ij1ocj</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>My Winter Nails + Color change</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij1ocj</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1ij8sgd</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Help i developed an allergy to gel nails</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nrok9xvg5khe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1ij8zvj</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>In time for Valentine's day💅 💕</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij8zvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1ij89u1</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>How dangerous are gels really? In regards to allergies?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ij89u1/how_dangerous_are_gels_really_in_regards_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1ij8ljs</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Valentine’s Nails</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mikxjwv14khe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1ij8d9g</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Valentine nails🎀💗</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stf3mbbc2khe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1ij88xk</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Natural nails breaking</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ij88xk/natural_nails_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1ij3d60</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>How does this look like?</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hipyrsyk0jhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1ij4837</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Help on starting acrylic</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ij4837/help_on_starting_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1ij82qa</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Recent Nail Designs</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij82qa</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1ij0w2w</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>How do I fill gel nails with artwork on?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3cwfnjhdihe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1iiwpob</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>HELP OPI gel reaction 😭</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiwpob</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1ij73ar</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Love my neon frenchies</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5rp0v56tjhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1ij6ad6</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Do you guys like the shape of my nails?</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6efdkldnjhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1ij65gb</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>First time trying Gel-X</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij65gb</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1ijq474</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Valentine’s nails (by me) ft. Chonky hearts</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2gmakjadohe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1ijpd6f</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>An attempt at amethyst marble</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5cym8p93ohe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1ijpc0d</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>The Dragon's Flame</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1o7t2vt2ohe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1ijns06</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Pretty good after almost a week of wear! (Mooncat)</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66s0n2xlknhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1ijn0es</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Terrible shrinkage help!</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijn0es</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1ijmb9o</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Laqueristas, it's cold outside</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l7ayrx2j5nhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1ijm691</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>{PR} Alternative Valentines Mani</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijm691</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1ijltyr</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>gradient galaxy nails 💖</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hm5uyl8v0nhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1ijlh32</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Sorry for the weird post! My hyponychium is exposed because I think I must've torn off part of my nail. It's super painful to the touch and my finger is red and throbbing. Any tips on how to trim back the Hyponychium and reduce swelling..?</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktycyz1gxmhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1ijl9qj</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>So I've been nervous to try thermals, but LynB convinced me ❄️</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijl9qj</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1ijl04c</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Red Carpet gel not fully curing?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lseu2h66tmhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1ijki8z</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Cracked Polish Cornea Killer</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijki8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1ijk0zi</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>I shouldn’t use this right? Purchased off amazon.</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3w1w2xf6kmhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1ijioo1</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Lyn B Designs— Go Fish</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijioo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1ijilc8</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>You inspired me to buy ILNP Flowerchild. Definitely a fun color for February!</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dmjwbef7mhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1ijiegv</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Cosmic polish is blowing my mind!</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijiegv</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1iji6at</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>ILNP Roulette velvet</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r9q71p0r3mhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1ijhbhs</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Zoya Adina</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ijhbhs/zoya_adina/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1ijh8pp</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>It's giving Sailor Moon! 🩷🌙 (+ big chop eulogy)</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijh8pp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1ijh45l</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>She gorgeous</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijh45l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1ijh2zf</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>BEHOLD</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mp58v46mulhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1ijgyqu</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>finally organized all my nail polishes</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kasmg97mtlhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1ijguy3</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>LynB Helix is amazing 💖</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijguy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1ijgfa8</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Favorite Luigi Green polishes?</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ute5f89dplhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1ijgd0z</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Drug store polish vs premium polish</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ijgd0z/drug_store_polish_vs_premium_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1ijfvjh</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>winter royalty vibes</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijfvjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1ijf36e</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>30th Birthday Nails!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijf36e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1ijeynt</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>If I got a manicure or a mani-pedi</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ijeynt/if_i_got_a_manicure_or_a_manipedi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1ijetei</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>i’m feeling Lavender Fields ♥️</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cd046jxyclhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1ijeste</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>A neutral skittle (or Reese’s Pieces?)</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijeste</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1ijenm9</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Three of the new Clionadh magnetics! Galerina, Inocybe, and Panaeolus</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijenm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1ijefpx</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Aurelia by Arcana Lacquer on natural nails</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijefpx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1ijecin</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Did I buy fake Nail Envy?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82ke236l9lhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1ijdke1</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Galentines Ready!</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13oo834y3lhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1ijdief</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Holo Taco DavidsTeal restock?</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ijdief/holo_taco_davidsteal_restock/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1ijcu8k</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Recommendations for toppers that look like this?</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clmlc7bqykhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1ijctq9</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Got married in Smokescreen</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myj0y6lmykhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1ijcl07</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>I think my bottle of smitten arrived tarnished?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijcl07</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1ijbwy0</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>My attempt at Hello Kitty nails</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijbwy0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1ijbkeg</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Deep Space</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijbkeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1ijb7hy</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Nail tools</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ijb7hy/nail_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1ijaxc8</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Forgot how much I like pink~</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijaxc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1ijawvu</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Cirque - Sugar Plum</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijawvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1ijafd5</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Comparison of Mooncat’s Blossom’s Firebreath (Powerpuff collection) vs Cirque’s Fairy Floss</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ijafd5/comparison_of_mooncats_blossoms_firebreath/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1ija8qc</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Probably one of the most eye catching polishes I own now</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/umxzp8oyfkhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1ija23m</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Do GITD polishes have a shelf life?</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ija23m/do_gitd_polishes_have_a_shelf_life/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1ij9rdv</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>BP sending out random lil care packages?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdo84qseckhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1ij9gta</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>The Village Chief</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij9gta</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1ij96dm</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Trans charity polishes?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvahvwm78khe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1ij8w6j</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>What's a nail polish you love wearing but hate removing?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ij8w6j/whats_a_nail_polish_you_love_wearing_but_hate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1ij8uck</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Hello Brother!</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij8uck</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1ij8rk1</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Help i developed an allergy!</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9qhlqw95khe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1ij81ku</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Valentine's, super simple</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij81ku</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1ij7lr9</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Love Witch 💕</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij7lr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1ij7kjg</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Lurid's Brunhilda is giving fabulous swamp witch!</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vv0jni9fwjhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1ij7akx</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Sometimes combos look way better in your head than they turn out IRL</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij7akx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1ij6vej</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Peony for your thoughts🩷💜💙</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij6vej</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1ij6ax2</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Forbidden Fruit, on for 1 week for my holiday in Thailand ⛱️💚</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij6ax2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1ij67z2</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>what are some of the easier ways to do nails at home? the only knowledge i have is from watching when i'd go to a salon, i've only ever gotten acrylic and dip.</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ij67z2/what_are_some_of_the_easier_ways_to_do_nails_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1ij66m3</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Chicago Fire</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/em3ef8xlljhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1ij5uj7</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Does the clock start ticking on Thermals when it's opened or when it's poured?</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ij5uj7/does_the_clock_start_ticking_on_thermals_when_its/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1ij5n5w</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>100% acetone before painting doubled the life of my manicure!</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/84xdaudoijhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1ij5fgr</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>ILNP Bluebell vs Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij5fgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1ij5bvb</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>🌋The Nails Are Lava🌋</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij5bvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1ij589e</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Imperial Stormtrooper</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij589e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1ij52t9</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Birefringence and deep space 🌠</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdki9v8bejhe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1ij4x5h</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Best QDTC for Jen&amp;Berries/BCB Flakie Polishes to avoid shrinkage?</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ij4x5h/best_qdtc_for_jenberriesbcb_flakie_polishes_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1ij32ch</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>💅🏾 When Your Nails Are That Good… Even the Nail Tech Had to Flex Them 💅🏾</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij32ch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1ij4cxz</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>I was feeling underwhelmed by this months PPU….</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ij4cxz/i_was_feeling_underwhelmed_by_this_months_ppu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1ij3m2u</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>💘Valentines Vibes 💘</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij3m2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1ij3j4r</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Frozen 🧊</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij3j4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1ij35lu</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>What's February without at least one Valentine's set?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij35lu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1ij34kn</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Nailboo, Manicurist Green Flash or Dazzle Dry?</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij34kn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1ij2p5s</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>There’s a Christmas Beetle in my Ice Cream! (First time order with IDU)</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij2p5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1ij1n5y</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Aus/ can someone recommend a physical store to buy chrome powder in Melbourne?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ij1n5y/aus_can_someone_recommend_a_physical_store_to_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1ij1ia3</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Red nails and fancy gloves</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij1ia3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1ij1dsm</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>In love! Very wintery</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij1dsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1ij13br</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Needed to show this sparkle!</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/54nck80hfihe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1ij0j62</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Ebay disappointment</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij0j62</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1iizrmz</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Normal topcoat on acrylics with gel overlay?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1iizrmz/normal_topcoat_on_acrylics_with_gel_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1iimsra</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>For the girlies with red hands</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lu3h09ydcehe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1iiy2bw</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>A queer take on valentines 🏳️‍🌈🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiy2bw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1iiy0nl</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Treasures or Bugs - LynB</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iiy0nl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1ijpgpe</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>At attempt at amethyst marble</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/beb5bu6k4ohe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1ijpgeu</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>The Dragon's Flame</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqrp2vfg4ohe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1ijlxjc</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Cherry</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pn5zc3u1nhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1ijorzy</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Almendras para el día de san Valentín ❣️❣️❣️</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zq3pau0svnhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1ijnakh</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Freehand art 🥰 how do you think it turned out?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ed97bfpifnhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1ijn466</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Expectation vs Reality</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijn466</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1ijmcip</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Ombré Glitter + Pink &amp; White Hearts</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcvfhyrv5nhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1ijmasb</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>4th set ever</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/affotmfe5nhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1ijm2fc</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Cat Eye Heart Fail?</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mclh6ne53nhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1ijlahi</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>I love them</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijlahi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1ijk8ir</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Been practicing with foils</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqe9wgm3mmhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1ijk2xm</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Love Day Set</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijk2xm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1ijilps</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Jinx/Arcane Inspired Set 💙</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yryhsxvi7mhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1ijh1ih</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>February Nails💌🎀💗❣️</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2wfexh7aulhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1ijgn5k</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Some cuties for Vday</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucxebxz2rlhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1ijdb1h</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Fairy magnetic nails</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijdb1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1ijd9l3</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Fun nails for February 💅🏽</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gyw9ks0u1lhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1ijbj6i</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxc5ruabpkhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1ijb4p1</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails 🩷</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0cygxwbmkhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1ij5bpp</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Helloo girls 💘 I do acrylic nails this some pictures about my job, I accept criticism!</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij5bpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1ij446y</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Tried to do something a bit more creative than usual</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij446y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1ij25n8</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>French nails pink 🥰</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij25n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1ij1bu0</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>aquarium nails!!</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ij1bu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1ij07ro</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Full Nail Art</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgcrqvtk5ihe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1ij078l</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>I made them to my friend. Advieces to improve</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pr0k18me5ihe1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Feb  8 08:09:27 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_09.xlsx
+++ b/data/collected_data/2025_02_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1088"/>
+  <dimension ref="A1:C1260"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18929,6 +18929,2930 @@
         </is>
       </c>
     </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1ikhtmz</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Nail glue options for allergy</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikhtmz/nail_glue_options_for_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1iki4oe</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Pink flames</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/catum2rudvhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1ikhz9q</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Anti valentines nails</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikhz9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1ikhxea</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Looking for a Nail Tech Mentor in North York!!</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikhxea/looking_for_a_nail_tech_mentor_in_north_york/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1ikhrw7</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Nail broken</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikhrw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1ikhqpd</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Hard Gel Valentine's Day nails</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ommxjpny8vhe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1ikh570</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Sad times</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rokkmo9v1vhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1ikg9n7</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Hoping these nails bring me some Valentine's luck! 😉</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmnbip4uruhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1ikhf64</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Malachite marbles w/ gelish blooming gel 💚</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h58jpv455vhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1ikhao2</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Gel x Feb. set🌸💖🌷🎀</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikhao2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1ikh449</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Where to buy somewhat cheap but good quality acrylic supplies?</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikh449/where_to_buy_somewhat_cheap_but_good_quality/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1ikgu4s</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Valentines nails 🩷</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8uj9dzayuhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1ikgtfw</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>🍒🍒🍒</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikgtfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1ikgfqy</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>How much would you pay for these valentine nails?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mtgo80tvtuhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1ikgf75</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Nail growth journey with builder gel</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39o34u3qtuhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1ikg58z</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Vegas Baby!</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikg58z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1ikfv75</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>My favorite Valentine's set</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikfv75</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1ikf94o</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Vday</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzp7jmrhhuhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1ikfbff</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>DIY Vday nails</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ex9c0de5iuhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1ikf7n3</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Did my nails for Valentine’s Day (Gel-X)!</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikf7n3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1ikf34b</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Gel Valentine’s Nail</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9652cnrfuhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1ikf28o</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Birthday Nails🩷</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikf28o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1ikesb8</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Russian manicure 💅 troughs?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikesb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1ikegzi</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>February Nails</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnrgdvvn9uhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1ikdkjy</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>How to get off glue on top of press ons?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikdkjy/how_to_get_off_glue_on_top_of_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1ikcu6l</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Love how these turned out!</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikcu6l/love_how_these_turned_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1ikdz8m</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Am I going crazy??</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikdz8m/am_i_going_crazy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1ikdv36</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Nail dump</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikdv36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1ikdu5d</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Valentines day nails 💕</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikdu5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1ikdn89</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>My nails are officially ready to take flight.</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmbbpsep1uhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1ikdh8d</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Gel with Fibers</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikdh8d/gel_with_fibers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1ikddc9</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>First time posting here</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikddc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1ikdc5g</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails 💕❤️💖💘</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlenqrqwythe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1ikd4nv</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>I’m not sure how I feel about these</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vixqeg30xthe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ikd48w</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Opinions?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zk2ecsjwwthe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1ikc8ej</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>A walk and pretty nails to lift my mood ✨</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eenu69quothe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1ikc0al</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Whimsical valentine nails</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94cr4k1vmthe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1ikbsau</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Tempted to ditch the dip….</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikbsau/tempted_to_ditch_the_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1ikbo5c</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Just wanna show off my incredible nail tech 🥹🤍</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikbo5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1ikbn3s</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Pretty in pink! 🌸 Age is 45, but still feels like a teenager</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikbn3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1ikbjia</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>So so happy how my Valentine’s nails turned out!</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahmjgc1nithe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1ikbio3</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Bday nails &amp; in the wild</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikbio3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ikbb3d</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>first time wearing press-ons as a guy</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z55p5b2mgthe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ikbacx</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>How bad are these gel x?</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8xby53egthe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1ikb76f</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Rain nails for myself this week 🌧💜</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikb76f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1ikavqn</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails! How’d I do?</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikavqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1ikaskf</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Why do nail techs keep pushing dip?!</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikaskf/why_do_nail_techs_keep_pushing_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1ikaosx</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Vday Goth Set 🖤</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bpcd219bthe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1ikaiyj</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Cat eye effect. What do you think of my new nails?</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikaiyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1ikae8d</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Loving my new set!</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikae8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1ikab12</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Did I pay too much? ($150)</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikab12</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1ika1g9</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>onycholysis help</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ika1g9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1ik9wjb</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>black polish with nail stickers i added ❥🙂‍↔️ sometimes i love rocking a short nail vibe.</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smy26e8n4the1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1ik9mxa</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Are those classy or looking cheap?</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8fswixj2the1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1ik9jjb</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Short, thin nails</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ik9jjb/short_thin_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1ik9gzk</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Princess Pink 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6sxvjzl61the1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1ik9gqk</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Russian pink-nude gel mani 🌷</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik9gqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1ik9glv</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Can you find the snake? Did not have a mold at hand so I had to do what I could do…</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84mtj2j31the1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1ik9brf</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Any recomendations for polishes with mirror effect (in EU)?</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ik9brf/any_recomendations_for_polishes_with_mirror/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1ik997b</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>3rd polygel set</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik997b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1ik93by</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Purple Vday nails 💜✨</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1k9hai1yshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1ik92w8</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Valentines Day Ready!!!</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4mibe2yxshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1ik6tyi</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Fresh Acrylic Nail Rash???</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik6tyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1ik89cl</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>I had a manicure today and am very happy with the result</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u28l8z9arshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1ik87fc</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Loving my new set!</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipnzf360rshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1ik719k</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>If I apply press ons with my nails in their current state- will I potentially contribute to developing a glue allergy?</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bzi2p8whshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1ik77x1</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>My second set + Valentine’s Day inspired. Still not comfortable doing nail art so all the pinks will have to do! 💗</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik77x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1ik6cx3</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>My boring ass nails (that I love)</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3q3id5vcshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1ik8164</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Trying out gel nails at home! I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7c5iwknpshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1ik7we9</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Took a chance on Amazon no-name brand press-on nails. Sizing is a bit off but I like them.</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik7we9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1ik7vo2</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Birthday Nails 💗do you see a pig or a cow🐽🐮</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21meno6hoshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1ik79h6</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Holographic</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wt33jvynjshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1ik752i</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Before and after Valentine's nail set ❤️</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik752i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1ik72yn</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Valentines Day Set &lt;3</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik72yn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1ik6w1c</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>notebook doodles on gel-x</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik6w1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1ik6ilk</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Valentines Day Nails ❤️</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ta0xgjp0eshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1ik6dhk</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Kingdom Hearts Sora Cover Art as Nail Art!</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik6dhk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1ik660s</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Working on my almond shaping</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8kf79n2ebshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1ik64q4</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Lover Girl</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7p3mxb4bshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1ik5c06</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>These took me 8 hours but it was so worth it! @nailsalon_lavie, @mythica_yuki &amp; @_akala_nail_ for inspo (swipe)</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik5c06</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1ik4zjd</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Flora inspired nails i did on myself</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fceh4kii2she1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1ik4g62</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>First time using nail polish. They look terrible.</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik4g62</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1ik57ah</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>❤️‍🔥 Name A More Perfect Red</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0tghqvi24she1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1ik4rgg</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>because i can’t do the trending magnetic heart nails even if my life depended on it 🤦🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nww7rtrs0she1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1ik4fs7</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Mexican pottery inspired nails</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spl94fgbyrhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1ik4n5e</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lm9g07lvzrhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1ik4jbq</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Why does my uv lamp do this?</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bl5p9vf1zrhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1ik4eek</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>One lamp? Many lamps? TOO many lamps?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ik4eek/one_lamp_many_lamps_too_many_lamps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1ik4crg</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Another day, another slay</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tc2mnd1oxrhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1ik477w</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Builder gel with a little stone🤍</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik477w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1ik442z</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails 💋</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik442z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1ik43pa</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Fresh for V-day ☺️</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lml22uztvrhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1ik3zox</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Pastel Goth nails</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rc5ovyhzurhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1ik3zko</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>I can't get the nail form to sit flush with my nail. Roast me!</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik3zko</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1ik3tme</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>nothing fancy i just think they’re cute</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik3tme</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1ik3r9j</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>First time!</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik3r9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1ik38oy</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Valentine's ❤️🩷</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akwcmv1dprhe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1ik36hu</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Vday Nails!</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik36hu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1ik2s5x</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>My nails aren’t staying on. Pls help!</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ik2s5x/my_nails_arent_staying_on_pls_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1ik30lz</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Valentine's Vampire Shine Nails</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik30lz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1ikhfij</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Dance With Me by Cuticula (Jan 25 PPU)</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikhfij</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1ikgooa</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Can I do gel nails outside?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ikgooa/can_i_do_gel_nails_outside/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1ikglip</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>(A Very Late) What I Wore in January</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikglip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1ikfvs4</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Can I Just Add Black to Darken Teal?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikfvs4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1ikeb6l</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>This brand has to be someone's vibe in here</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ikeb6l/this_brand_has_to_be_someones_vibe_in_here/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1ikcpow</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>My nails are so weak and peely, to motivate myself if I oil them 3x a day for 1 week I'm going to buy myself my 1st indie polish, if I do it for a whole month I'll buy a collection</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikcpow</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1ikbbms</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Cute V-day manicure or… Salami Fingers?!</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikbbms</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1ikavhm</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>November - January purchases before the no buy 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikavhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1ika0n8</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Friday mood</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zio7j7wk5the1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1ik9o30</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Urgent: de-influence me from buying 200$ worth of Starrily</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ik9o30/urgent_deinfluence_me_from_buying_200_worth_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1ik9ma3</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Holo Taco - Toe Beans 🐾 🩷 to kick off a month of pink manis</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik9ma3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1ik93i4</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Playing around with gel polish layers and sanding</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nukha853yshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1ik8wxn</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Thoughts on quick dry polish?</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ik8wxn/thoughts_on_quick_dry_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1ik8wto</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Box of Chocolates</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik8wto</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1ik8r3r</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>best white for french tips?</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ik8r3r/best_white_for_french_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1ik8e4x</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>the seven ravens ✨</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik8e4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1ik8chh</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>My first attempt at velvet bails</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ao9bpmu2sshe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1ik81u0</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Love the polish &amp; the reference, but...</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik81u0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1ik7srr</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Non-gel chrome powder nails - think I finally, really cracked the code!!!</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6v7jv2rrnshe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1ik7ssw</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>How do we feel about dips?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik7ssw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1ik7dfv</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Dupe for Lurid's "Schneewittchen"</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ik7dfv/dupe_for_lurids_schneewittchen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1ik7826</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Producer recommendations for a beginner</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ik7826/producer_recommendations_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1ik6moh</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Chipping already</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ik6moh/chipping_already/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1ik6js3</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Making the best of a major nail break and chop! 🥰❤️💕</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik6js3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1ik6d50</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Alien Invasion 👽</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik6d50</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1ik5gi2</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Manis as of late</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik5gi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1ik4zas</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>❤️‍🔥 Name a more perfect red.</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/paaquj6f2she1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1ik3kxp</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Gloomy winter nails did not match the weather today ☀️</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68eeknevrrhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1ik39s2</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>blown away by my very first indie!</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik39s2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1ik2w3h</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>ILNP - Deep Space</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik2w3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1ik2sor</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>I couldn’t believe my eyes</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9e9r4ut0mrhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1ik2p0l</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>classic valentines manicure</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik2p0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1ik215a</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Tips to make very short nails look good?</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ik215a/tips_to_make_very_short_nails_look_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1ik1y0s</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>I just tried Bees Knees Lacquer for the first time and I’m in love! 😍😍😍</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik1y0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1ik1qny</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Classic red on shorties = love ❤️</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik1qny</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1ik1lkv</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>To Teach Us about Our Past</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik1lkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1ik1j6a</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Holo to celebrate Helios 🌞</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik1j6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1ik0sxb</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>ILNP Deep Space</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik0sxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1ik0jtr</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Zoya Adina (Second attempt)</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik0jtr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1ik07h9</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Feeling moody with Cracked’s “Vamped Vanity”</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik07h9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1ijzw2n</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Purple gel nail polish recommendations</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ijzw2n/purple_gel_nail_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1ijzq0z</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Valentine’s Day 2025 Mani #2</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s62gmbtqzqhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1ijznak</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>chrome came off after wearing vinyl gloves</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijznak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1ijyj3o</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>thoroughly obsessed.🦕</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhoey32xqqhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1ijygrn</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Was there an indie drop last night at 9pm?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ijygrn/was_there_an_indie_drop_last_night_at_9pm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1ijxpbf</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Doing a gradient is too much hassle</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijxpbf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1ijwy5w</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Another Valentine's Mani</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/syud917weqhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1ijwhy2</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Help growing nails (silk or fiberglass nail wraps)</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ijwhy2/help_growing_nails_silk_or_fiberglass_nail_wraps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1ijvkci</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Back at it again with the comparisons 🙈</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijvkci</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1ijv6a3</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>A perfect neon lavender</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijv6a3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1ijt6v6</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>How can I fix this? I've never had a nail break this badly :(</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9v9a7p8gphe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1ijqcbr</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Nabyo — Kirara. A stunning magnetic turquoise 🩵✨</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijqcbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1ikgdet</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>some sets from jan/feb</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikgdet</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1ikg22m</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Love how these turned out</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikg22m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1ikexsx</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Winter Nails + Color change</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikexsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1ikewqp</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Liza frank, 80es inspired nail set</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikewqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1ikefhz</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Valentines Day Nails</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikefhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1ikdsh0</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>my girl did that‼️‼️👁️👄👁️</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikdsh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1ikcyn7</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>I tried to make realistic pie/ bakery nails</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ps408gwfvthe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1ikbdbz</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>i dont know what to do with this pink nail</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eu76a6r5hthe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1ika2ak</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Valentine’s set ❣️</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/saqvptyy5the1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1ik9to4</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>thoughts ? price estimate ?</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik9to4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1ik8qma</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Fav mani</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbnu4ks8vshe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1ik6r4i</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Looked better in my mind</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xs3xzvosfshe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1ik60tf</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>February ❤️</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik60tf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1ik4ga9</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Hand painted on my own nails</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik4ga9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1ik47qy</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>La Lidia ❤️</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22pi5m9nwrhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1ik0sku</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Which nail design should I go for?</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ik0sku/which_nail_design_should_i_go_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1ik0036</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Pink &amp; red stripes hand painted on myself 🩷❤️💅🏼</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ik0036</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1ijzd02</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Beginner Looking For Critiques and Feedback!</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ijzd02</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1ijycho</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>custom press ons</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hkl2hybkpqhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1ijxl9o</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>I like to look for Nail Art designs and recreate them, do you like me?  You can leave me another design in the comments to complete the challenge 🤣</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzzewfzwjqhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Feb  9 08:09:41 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_02_09.xlsx
+++ b/data/collected_data/2025_02_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1260"/>
+  <dimension ref="A1:C1455"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21853,6 +21853,3321 @@
         </is>
       </c>
     </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1il9exd</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Pretty nails, happy me.</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il9exd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1il98ga</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Any ideas on how to add glitter onto this color?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il98ga</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1il90ti</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Hand painted Year of the snake nail art</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pcfvj8fka2ie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1il8sw3</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Red valentine perfection</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0xxsans72ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1il8quc</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>My nail tech wanted to try out her new acrylic powder on me</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il8quc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1il8okt</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Are there any sculpted gel-x tips that aren’t apres?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1il8okt/are_there_any_sculpted_gelx_tips_that_arent_apres/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1il8nk8</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Blue and pink ombré nails oh</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8azsuzs062ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1il82m8</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Gummy bears nails 💜</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12g4amy7z1ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1il80iw</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>My Valentine’s set.</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il80iw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1il7vfl</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>My V-Day Nails🤩♥️💖</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il7vfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1il7o4z</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>almond vs square</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il7o4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1il71dc</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>i got bored so i freestyled these valentines themed nails 😝</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5qede0zn1ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1il6ott</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Are these too thick?</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il6ott</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1il6moy</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>What colour does this look like to you guys?</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g5w4qluoj1ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1il5ypc</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Need help with nail shaping</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5g0wr3pyc1ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1il5fso</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Simple vday set</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ldfz3cp71ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1il571k</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Barbie girl 💅</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rpf7pgc51ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1il53mv</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>in honor of the month of love, Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zefeg5tg41ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1il4yy4</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Did cat eye myself</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il4yy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1il11k4</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Nail cracked each side</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il11k4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1il468f</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>cleaning up french tip, polish spreads</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1il468f/cleaning_up_french_tip_polish_spreads/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1il4dc0</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Press-ons for clubbed nails?</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1il4dc0/pressons_for_clubbed_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1il4voc</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Would it be weird to leave my hands uneven?</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il4voc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1il4u6a</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>KISS Galaxy</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il4u6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1il4to1</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Not too fancy, just right for my birthday.</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il4to1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1il4sg3</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>My first set ever!</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/csno9lqh11ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1il4oux</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Question about nail shape</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0psx61k01ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1il4e1j</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>❤️🩷</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3g1onh0px0ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1il413y</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>my friend did them!</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7iqiu6du0ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1ikq2ht</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>How can i prevent this?</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikq2ht</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1ikzeh0</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Soft but original nails?</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikzeh0/soft_but_original_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1il34s2</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>My gel keeps peeling at the cuticle area?</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2iom5jf5m0ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1ikzywo</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Thanks for the inspiration :)</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cl8cn7l3vzhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1il3891</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Baby Nail Tech here needing some help</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1il3891/baby_nail_tech_here_needing_some_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1il3mxd</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Newbie to gel nails and have a (maybe dumb) question</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1il3mxd/newbie_to_gel_nails_and_have_a_maybe_dumb_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1il3lh8</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Noho Nails?</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvfg5msdq0ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1il3a8i</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>V-Day nails!</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il3a8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1il349d</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Shape suggestions please!</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il349d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1il2st3</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>American Manicure</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il2st3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1il2jih</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>I don’t know what my expectations should be</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il2jih</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1il2hy9</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Nail technicians, help!</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il2hy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1il20ps</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>3rd times a charm</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il20ps</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1il1z51</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Never had red nails until today!</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rct7o2oub0ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1il1wzy</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>white part of nail seems to be extending down?</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9t5gkr6cb0ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1il1sse</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails ❤️🩷</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84eqmhrba0ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1il1n1e</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>What color may I choose?</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1il1n1e/what_color_may_i_choose/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1il1izt</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Classy &amp; Sparkly</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goq2lc5z70ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1il1hl8</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Set my friend did for me!</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il1hl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1il0r69</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Removed gel in the worst way possibile now my nails are ruined</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1il0r69/removed_gel_in_the_worst_way_possibile_now_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1il0nq3</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set I did at home!</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il0nq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1il0dxn</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>These are my first nails that I do, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yalv7yxfyzhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1il09w8</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Que tal este tono rojo ❤️, les gusta? O prefieren algo más vino</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il09w8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1ikzwxx</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>My first ever Valentine’s Day set 🩷💅</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xv05o76nuzhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1ikyumq</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Valentine's day nails</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikyumq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1ikyn9o</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Balatro nails? Or siren nails🤣🚨</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06d7mjykkzhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1ikxlp5</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Having issues with polish lasting.</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikxlp5/having_issues_with_polish_lasting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1ikx9o3</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Looking for a dupe</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0f4bkv9s9zhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1ikwssx</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>No one talks about how nail fungus destroys your confidence, not just your feet.</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikwssx/no_one_talks_about_how_nail_fungus_destroys_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1ikz4o0</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Beginner gel nails, how’d I do?tips for improvement?</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h43krtdozhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1ikz2xr</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Cat eye, 2nd try !</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikz2xr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1ikyvaw</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Bump from nail tip</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikyvaw/bump_from_nail_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1ikyfop</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>obsessed with my manicure today</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2dtqw1sizhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1ikyev8</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Can’t wait for spring … 🦋✨</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikyev8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1iky676</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>fresh set 🤍🥰</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8oba9hsgzhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1iky5dv</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Hoping nobody's tired of Valentine's nails yet 💖</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3pe0swlgzhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1iky0jc</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>My first Valentines set</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iky0jc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1ikxywg</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Best friend’s wedding is next week. HELP!</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikxywg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1ikxxsc</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Added some stones for fun!</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6p5oviyezhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1ikxpaj</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>How to go about doing gel nails with curved nails?</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikxpaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1ikxc5i</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Nails I’ve done as a hard gel specialist on natural nails recently 💕</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikxc5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1ikx5nl</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Bridal wedding nails</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f59d3u6x8zhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1ikx5bf</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>the cat eye polish was so pretty 😍</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fn1xwzsu8zhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1ikx4el</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Valentine’s mani</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2me8m0qn8zhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1ikx3lv</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>made a set in time for Valentine’s Day 🥰</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wl1ql1fh8zhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1ikwzoh</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Weekend set</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ux5e92tl7zhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1ikwc95</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Humming bird Chopard set</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikwc95</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1ikw0ly</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Did these bad girls today 🥹</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9q2svhb30zhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1iklk0r</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Pigmented and darks colors are not curing correctly</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1iklk0r/pigmented_and_darks_colors_are_not_curing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1ikvyk5</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Valentines day set</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4se3nd7nzyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1ikvyip</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Butterfly cat eye!</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0oz65grmzyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1ikn59x</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>What should I do with a nail that's already peeling?</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikn59x/what_should_i_do_with_a_nail_thats_already_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1ikvagb</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Valentine‘s day Nails ❤️🌹              #inspo</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6v1nlzmjuyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1ikti5c</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>How 'durable' is nail polish? (aka what can ruin nail polish?)</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikti5c/how_durable_is_nail_polish_aka_what_can_ruin_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1iksh7r</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>how do i do them at home</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbrjwzfk9yhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1ikvs67</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Valentines Set 💕</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5mczrg99yyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1ikvfvd</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>What's wrong</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikvfvd/whats_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1ikv57z</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Press ons with sticky tabs moving</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikv57z/press_ons_with_sticky_tabs_moving/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1ikt7e8</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Beetles gel polishes</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ikt7e8/beetles_gel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1ikt8we</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Trying Essie gel couture; what do you think?</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qki30ucfyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1ikumkc</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Does anyone have any idea why my nails are like this? My nails also are VERY thin once they grow out and almost always have these lines…</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bi52ouplpyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1ikulhe</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Li’l Valentine 😍🦉💞</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qa1ukccepyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1ikuc1d</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Love Letters and Trinkets</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikuc1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1iku878</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Feels good to have claws again ❤️</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iku878</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1iktwcb</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>My valentines set ❤️</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtajv6c5kyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1iktvbi</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>I love my valentine nails 💌</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iktvbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1iktl1q</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>I did these for my first ever set in myself. Junk nails.. 🙃💗 I think they’re cute</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nskwsvrhyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1iktclw</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Octopus nails 🤎</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iktclw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1ikt87n</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>My Valentines Day set🩷</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikt87n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1ikt2ms</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Last Valentine’s Day set❤️</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99622pk1eyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1ikt24g</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Brown with blue chrome ✧･ﾟ: *✧･ﾟ:*</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d278x3ydyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1il9rto</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>How to not get chrome to chip? 🥹</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1il9rto/how_to_not_get_chrome_to_chip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1il7l2a</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Coordinating with my mani</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kuagwwjvt1ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1il7dg3</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Mooncat - Sealed With A Hiss mani!</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1il7dg3/mooncat_sealed_with_a_hiss_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1il7afa</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Fun nails for valentines/a friends birthday!</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q0btcugnq1ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1il79ey</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Clean and simple 🧼</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cec5khzcq1ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1il79d8</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Flakies x parking lot lighting</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il79d8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1il72b0</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Cirque Lyra</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ob6j0jz6o1ie1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1il6uew</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>So impressed ...</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/P7KimHO</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1il6irl</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>I found this insanely beautiful seashell at a shop and now I’m wondering if there’s a nail polish color that looks like this?</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9addb2dki1ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1il6emn</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Spouse went a snack run, came back with this</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/400ryoidh1ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1il6alz</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>$2 Nail Polish For The Win!</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il6alz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1il644w</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>A little valentines mani!</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il644w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1il5h7h</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>She's a wild-flower child</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il5h7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1il491w</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Purple hearts vday bling</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il491w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1il3zs4</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>custom buttons painted with nail polish</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahh4la1zt0ie1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1il3n85</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Magnetic Polish vs Magnetic Gel Polish</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1il3n85/magnetic_polish_vs_magnetic_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1il3kf2</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>LOVE my new Sally Hansen's Insta-dry Red!! Goes on smooth, dries fast and looks great! Especially when I top it with Sally's Hard As Nails!!</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u17emywwp0ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1il3ca8</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>But Daddy I Love Him</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il3ca8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1il383t</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Orly’s new Acid Trip - such a fun glitter!</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il383t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1il26i7</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Arcana Lacquer - “Ashes of Creation”❤️‍🔥 Instagram keeps removing the first photo from this post &amp; it’s bumming me out because it was my favorite.</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il26i7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1il2572</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Cock-a-Doodle-Doom 💜❤️</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mtfwnovbd0ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1il1h1m</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Super disappointed in PPU polish inspirations/descriptions</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1il1h1m/super_disappointed_in_ppu_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1il12o9</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>First time trying tortoise print</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il12o9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1il11nv</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>How do you "wrap the tips"?</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1il11nv/how_do_you_wrap_the_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1il0xue</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Is there a way to magnetize so that the magnetic particles don't show?</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bg6lke7x20ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1il0t4p</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>In love with ILNP Flower Child!</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8jf4jlu10ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1il0nb6</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Removing press on nails?</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1il0nb6/removing_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1il0jdn</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>I Still Do …love this polish :)</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il0jdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1il0gjc</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Shiftiest shifter ever?</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il0gjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1il0fd8</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>BKL Blade of the Frontiers</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il0fd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1il063t</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Magnetic Polish Particles Dispersing</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1il063t/magnetic_polish_particles_dispersing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1ikzljk</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>The most famous polish I know 💙✨</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikzljk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1ikzcda</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Serenity 💙</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikzcda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1ikz61q</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Vampy Valentines nails</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cluz1k6pozhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1ikz2g7</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Arcana Lacquer - “Emissary of Inari” from the Beyond the Myth collection (available 2/14 @6pm EST) 🦊♥️🩷</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikz2g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1ikylw3</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>✨️🌈Rainbow Watermarble🌈✨️</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikylw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1ikyg2o</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>First time trying out magnetic polish... I'm pleased!</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oatkr5nzizhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1ikx9lo</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Abomination Cosmetics Frost Topper</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikx9lo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1ikx720</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Can I use gel polish topped with a cat eye polish using a magnet? Appreciate the help.</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ikx720/can_i_use_gel_polish_topped_with_a_cat_eye_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1ikx4n9</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Seasonal Depression with a touch of regular depression</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1aez2sjp8zhe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1ikx3bs</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>My essie “lilacism” has become blue with time 😅 Is it just me?</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikx3bs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1ikw7go</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>I'm a sucker for a shifty shimmer 💚💙💜</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikw7go</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1ikvquk</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>ILNP Cross My Heart</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/r2JtKrH.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1ikvhfb</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Looking for a dupe polish for these Olive &amp; June press ons</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqumbra0wyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1ikvekm</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>How messed up are my nails and what can I do to help them?</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxgpvycfvyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1ikuz97</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Asked my boyfriend to pick the colours for my Valentine's week mani. Not convinced he understood the assignment 😂</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/704rayi7syhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1iktsh3</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Kinda speechless at this polish 🤯</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pn286b3bjyhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1iktool</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Trippy nails - cool from a distance, awful zoomed in</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iktool</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1iktn96</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>My "Valentine's Day" thermal is giving Nosferatu</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iktn96</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1ikt2xm</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Water based top coat?</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ikt2xm/water_based_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1ikszx7</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>Anyone successfully grow natural nails with nail wraps?</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ikszx7/anyone_successfully_grow_natural_nails_with_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1iksyrk</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Pretty Pandora</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iksyrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1iks9mq</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Asked my boyfriend to pick colours for me 🩷🧡</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iks9mq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1iks2zr</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>My first magnetic. Deep Space!</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b68hjn6l6yhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1ikrwre</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Birthstones on my nails 🤍</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikrwre</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1ikq7bm</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Trying hard to go on a no-buy, utterly failing this month</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zp2edomasxhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1ikps8p</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Help find similar color plz</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.oznailsbeauty.com.au/billionaire-gel-lacquer-duo-118-sweeties-15ml?srsltid=AfmBOor0oKwGz00aYcfL5xFlevmEGlkjQHxIw0c0TIuthV7PyeOe8bKR</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1ikpebb</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>this topper is like magic 🤩</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikpebb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1ikoa3p</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Need advice swapping from gel to normal polish</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ikoa3p/need_advice_swapping_from_gel_to_normal_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1ikllkn</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Mainstream Linear Holos - Looking to make a more complete list</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ikllkn/mainstream_linear_holos_looking_to_make_a_more/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1ikc2e4</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>My first PPU order</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ikc2e4/my_first_ppu_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1ijvhx6</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Soft and bending nails</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ijvhx6/soft_and_bending_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1ijzfh8</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Tips for preventing chipping on short nails?</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ijzfh8/tips_for_preventing_chipping_on_short_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1ikkrso</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>My Polish is on a Midwestern Tour</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5574wfdbwhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1ikkqtr</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>My nails have (literally) never been this long in my life</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qoudbc0bwhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1ikk04w</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Indie Brand Reputations List?</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ikk04w/indie_brand_reputations_list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1ikjpqh</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Velvetised Battery Check</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pgoqd0hvxvhe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1ikjbbk</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>Help my friend please</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ikjbbk/help_my_friend_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1il9s4e</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>Coco nails, oct 24</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il9s4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1il6pfc</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>V Day set!</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6gq1ozgk1ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1il67oq</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>first set on myself in years</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clzjj0yef1ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1il5g8w</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>Valentine's Day Cuties ❤️</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il5g8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1il4tf3</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il4tf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1il4nw2</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>I remember some nails I did for a friend when we lived in Brazil... what did you think of this design?</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86pq8dw901ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1il3sr2</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>17f Been doing nails for a while. Pls give me advice on how I can improve :)</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il3sr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1il2x5p</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Luigi nail stickers</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dalljdu7k0ie1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1il2j2l</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Not perfect, but still cute:)</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1il2j2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1ikzcpp</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>something sweet 🤎🍫</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikzcpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1ikylu5</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>World Nails - Can you guess the landmarks?</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikylu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1ikyjdu</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Valentines</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/urf4r2gpjzhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1ikwye2</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>My hand painted tiger nails for Vegas !</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/of17y29c7zhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1ikwenl</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Humming bird Chopard set</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikwenl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1ikwb1q</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Finally made some Year of The Snake nails!</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikwb1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1ikw4nt</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>I finally finished it💕💌</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikw4nt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1ikvxtr</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>I love this one so much it just so etherial, Ice fairy vibe! It not the best but the vibe is what do you think?</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikvxtr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1ikuhw0</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Took me a while but worth!</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k91o87zloyhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1iku77t</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Love Letters and Trinkets</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iku77t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1iksxwj</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Pencil Design for a Teacher</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cb5x63g1dyhe1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1iksozb</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>Emo Lumberjack</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1iksozb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1ikrzm9</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Supporting my best friend &lt;3 @clawedbydeia_</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikrzm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1ikqktb</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>We continue practicing pulse 🥰 what do you think of this design?</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4bd55lu6vxhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1ikofch</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>Valentines Set 💘</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikofch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1ikn9y4</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>2nd attempt at nail art!</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7k3hddjd3xhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1ikmo83</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Wife pink nails 💕</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aaf8x47hxwhe1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1ikjad4</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>Valentine's week nails</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ikjad4</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>